<commit_message>
server: add lost file
</commit_message>
<xml_diff>
--- a/Conf/Hero.xlsx
+++ b/Conf/Hero.xlsx
@@ -73,9 +73,6 @@
     <t>MP</t>
   </si>
   <si>
-    <t>Speed</t>
-  </si>
-  <si>
     <t>int(a)</t>
   </si>
   <si>
@@ -127,6 +124,10 @@
   </si>
   <si>
     <t>int(a)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SPEED</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -693,7 +694,7 @@
   <dimension ref="A1:O5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -756,7 +757,7 @@
         <v>11</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.15">
@@ -776,81 +777,81 @@
         <v>18</v>
       </c>
       <c r="F2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="H2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="N2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" t="s">
         <v>31</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="O2" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>21</v>
-      </c>
       <c r="C3" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M3" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N3" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="O3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.15">

</xml_diff>